<commit_message>
Augmented system LPF method
</commit_message>
<xml_diff>
--- a/Python/LPF_polyhedron.xlsx
+++ b/Python/LPF_polyhedron.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="64">
   <si>
     <t>it</t>
   </si>
@@ -46,43 +46,37 @@
     <t>[0. 2. 0. 1.]</t>
   </si>
   <si>
-    <t>[0.6268 0.2799 1.5605 2.7204]</t>
-  </si>
-  <si>
-    <t>[0.6391 0.5604 0.9618 2.4396]</t>
-  </si>
-  <si>
-    <t>[0.3301 1.3244 0.3608 1.6756]</t>
-  </si>
-  <si>
-    <t>[0.2284 1.5546 0.2054 1.4454]</t>
-  </si>
-  <si>
-    <t>[0.0667 1.8677 0.0644 1.1323]</t>
-  </si>
-  <si>
-    <t>[0.0167 1.9657 0.0185 1.0343]</t>
-  </si>
-  <si>
-    <t>[0.0145 1.9711 0.0144 1.0289]</t>
-  </si>
-  <si>
-    <t>[0.0103 1.9793 0.0103 1.0207]</t>
-  </si>
-  <si>
-    <t>[0.0083 1.9834 0.0083 1.0166]</t>
-  </si>
-  <si>
-    <t>[0.0016 1.9968 0.0016 1.0032]</t>
+    <t>[0.4461 0.8169 1.0287 2.1834]</t>
+  </si>
+  <si>
+    <t>[0.5094 0.8708 0.7304 2.1292]</t>
+  </si>
+  <si>
+    <t>[0.4622 1.0665 0.4803 1.9335]</t>
+  </si>
+  <si>
+    <t>[0.1836 1.6519 0.1455 1.3481]</t>
+  </si>
+  <si>
+    <t>[0.0052 1.9825 0.0195 1.0175]</t>
+  </si>
+  <si>
+    <t>[0.0135 1.9732 0.0129 1.0268]</t>
+  </si>
+  <si>
+    <t>[0.0044 1.9912 0.0044 1.0088]</t>
+  </si>
+  <si>
+    <t>[0.0039 1.9921 0.0039 1.0079]</t>
   </si>
   <si>
     <t>[0.0008 1.9984 0.0008 1.0016]</t>
   </si>
   <si>
-    <t>[0.0006 1.9987 0.0006 1.0013]</t>
-  </si>
-  <si>
-    <t>[0.0001 1.9998 0.0001 1.0002]</t>
+    <t>[0.0006 1.9988 0.0006 1.0012]</t>
+  </si>
+  <si>
+    <t>[0.0002 1.9995 0.0002 1.0005]</t>
   </si>
   <si>
     <t>[0.0001 1.9999 0.0001 1.0001]</t>
@@ -94,40 +88,37 @@
     <t>[0.5 0.  0.5 0. ]</t>
   </si>
   <si>
-    <t>[1.2747 0.9694 0.7583 0.453 ]</t>
-  </si>
-  <si>
-    <t>[0.4732 0.1437 0.4911 0.1616]</t>
-  </si>
-  <si>
-    <t>[0.5389 0.1577 0.513  0.1318]</t>
-  </si>
-  <si>
-    <t>[0.4543 0.0444 0.4848 0.0749]</t>
-  </si>
-  <si>
-    <t>[0.4599 0.0114 0.4866 0.0381]</t>
-  </si>
-  <si>
-    <t>[0.4891 0.0046 0.4964 0.0118]</t>
-  </si>
-  <si>
-    <t>[0.495  0.0036 0.4983 0.007 ]</t>
-  </si>
-  <si>
-    <t>[0.4963 0.0026 0.4988 0.0051]</t>
-  </si>
-  <si>
-    <t>[0.497  0.0021 0.499  0.0041]</t>
-  </si>
-  <si>
-    <t>[0.4993 0.0004 0.4998 0.0009]</t>
+    <t>[0.8572 0.59   0.6191 0.3519]</t>
+  </si>
+  <si>
+    <t>[1.0073 0.5775 0.6691 0.2394]</t>
+  </si>
+  <si>
+    <t>[0.465  0.0876 0.4883 0.1109]</t>
+  </si>
+  <si>
+    <t>[0.4175 0.0114 0.4725 0.0664]</t>
+  </si>
+  <si>
+    <t>[0.4697 0.0048 0.4899 0.025 ]</t>
+  </si>
+  <si>
+    <t>[0.4957 0.0033 0.4986 0.0062]</t>
+  </si>
+  <si>
+    <t>[0.4982 0.0011 0.4994 0.0023]</t>
+  </si>
+  <si>
+    <t>[0.4986 0.001  0.4995 0.0019]</t>
   </si>
   <si>
     <t>[0.4997 0.0002 0.4999 0.0004]</t>
   </si>
   <si>
-    <t>[0.4998 0.0002 0.4999 0.0003]</t>
+    <t>[0.4998 0.0001 0.4999 0.0003]</t>
+  </si>
+  <si>
+    <t>[0.4999 0.0001 0.5    0.0001]</t>
   </si>
   <si>
     <t>[-7.5 -2.5]</t>
@@ -139,15 +130,15 @@
     <t>[-0. -0.]</t>
   </si>
   <si>
+    <t>[ 0. -0.]</t>
+  </si>
+  <si>
     <t>[-0.  0.]</t>
   </si>
   <si>
     <t>[0. 0.]</t>
   </si>
   <si>
-    <t>[ 0. -0.]</t>
-  </si>
-  <si>
     <t>[-0.75 -0.75 -0.75 -0.75]</t>
   </si>
   <si>
@@ -163,49 +154,46 @@
     <t>[-0. -0.  0.  0.]</t>
   </si>
   <si>
+    <t>[0. 0. 0. 0.]</t>
+  </si>
+  <si>
     <t>[ 0. -0.  0.  0.]</t>
   </si>
   <si>
     <t>[-0.  0.  0.  0.]</t>
   </si>
   <si>
-    <t>[0. 0. 0. 0.]</t>
-  </si>
-  <si>
-    <t>[0.799  0.2713 1.1833 1.2324]</t>
-  </si>
-  <si>
-    <t>[0.3024 0.0805 0.4723 0.3941]</t>
-  </si>
-  <si>
-    <t>[0.1779 0.2089 0.1851 0.2209]</t>
-  </si>
-  <si>
-    <t>[0.1038 0.0691 0.0996 0.1083]</t>
-  </si>
-  <si>
-    <t>[0.0307 0.0212 0.0313 0.0431]</t>
-  </si>
-  <si>
-    <t>[0.0082 0.0089 0.0092 0.0122]</t>
-  </si>
-  <si>
-    <t>[0.0072 0.0072 0.0072 0.0072]</t>
-  </si>
-  <si>
-    <t>[0.0051 0.0051 0.0051 0.0052]</t>
-  </si>
-  <si>
-    <t>[0.0041 0.0041 0.0041 0.0041]</t>
-  </si>
-  <si>
-    <t>[0.0008 0.0008 0.0008 0.0009]</t>
+    <t>[0.3824 0.482  0.6369 0.7684]</t>
+  </si>
+  <si>
+    <t>[0.5131 0.5029 0.4887 0.5097]</t>
+  </si>
+  <si>
+    <t>[0.2149 0.0934 0.2345 0.2145]</t>
+  </si>
+  <si>
+    <t>[0.0767 0.0188 0.0687 0.0895]</t>
+  </si>
+  <si>
+    <t>[0.0024 0.0096 0.0096 0.0254]</t>
+  </si>
+  <si>
+    <t>[0.0067 0.0065 0.0064 0.0063]</t>
+  </si>
+  <si>
+    <t>[0.0022 0.0022 0.0022 0.0023]</t>
+  </si>
+  <si>
+    <t>[0.002 0.002 0.002 0.002]</t>
   </si>
   <si>
     <t>[0.0004 0.0004 0.0004 0.0004]</t>
   </si>
   <si>
     <t>[0.0003 0.0003 0.0003 0.0003]</t>
+  </si>
+  <si>
+    <t>[0.0001 0.0001 0.0001 0.0001]</t>
   </si>
   <si>
     <t>-2.50000</t>
@@ -575,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -621,22 +609,22 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H2">
-        <v>7.770727681979428e-17</v>
+        <v>3.024317889931462e-15</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -644,28 +632,28 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3.48496323918123</v>
+        <v>2.268766510013962</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H3">
-        <v>0.7700299671998959</v>
+        <v>0.2945409718455146</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -673,28 +661,28 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.249366762397172</v>
+        <v>2.014358062194479</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H4">
-        <v>0.2934541946221467</v>
+        <v>0.01869482220673623</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -702,28 +690,28 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.7927855267230781</v>
+        <v>0.7573123261747887</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H5">
-        <v>0.03486868424784317</v>
+        <v>0.1119533814054404</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -731,28 +719,28 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.3807217097655746</v>
+        <v>0.2537243339043396</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H6">
-        <v>0.03074629041765135</v>
+        <v>0.05358102995493548</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -760,28 +748,28 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.1263820875106909</v>
+        <v>0.04700182010186649</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H7">
-        <v>0.01552999586605267</v>
+        <v>0.01684186783593322</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -789,28 +777,28 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.03847496311827414</v>
+        <v>0.02597616108673728</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H8">
-        <v>0.003071710834298674</v>
+        <v>0.000282648487950674</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -818,28 +806,28 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.02867777672721905</v>
+        <v>0.008894441525290508</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H9">
-        <v>3.065057329645392e-05</v>
+        <v>8.350439583176112e-05</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -847,28 +835,28 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.02056040150968141</v>
+        <v>0.007859171913559448</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H10">
-        <v>1.900578361705664e-05</v>
+        <v>3.756441749740604e-07</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -876,28 +864,28 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.01650525838976602</v>
+        <v>0.00156601518440036</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H11">
-        <v>4.806368198673331e-06</v>
+        <v>1.163475132073282e-05</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -905,28 +893,28 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.003241751448909147</v>
+        <v>0.00116751312079999</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H12">
-        <v>5.119028937083206e-05</v>
+        <v>5.088339382860341e-08</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -934,28 +922,28 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.001579296631907479</v>
+        <v>0.000481811687263356</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H13">
-        <v>8.720774579548347e-07</v>
+        <v>1.392276209586947e-07</v>
       </c>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -963,28 +951,28 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.001254852758623359</v>
+        <v>0.0001093110860881374</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="H14">
-        <v>3.139206740016044e-08</v>
+        <v>4.115738851608374e-08</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -992,28 +980,28 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.0001720801583242615</v>
+        <v>6.896246543841578e-05</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H15">
-        <v>3.470868905669546e-07</v>
+        <v>4.876686656124749e-10</v>
       </c>
       <c r="I15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1021,28 +1009,28 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.0001045988318739699</v>
+        <v>1.458799371412134e-05</v>
       </c>
       <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H16">
-        <v>1.398136620478293e-09</v>
+        <v>8.765127689629989e-10</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1050,28 +1038,28 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>5.080497891229996e-05</v>
+        <v>1.191454383975277e-05</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H17">
-        <v>8.579783715243386e-10</v>
+        <v>2.207906056958755e-12</v>
       </c>
       <c r="I17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1079,28 +1067,28 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>3.223684895847789e-05</v>
+        <v>6.551690806322341e-06</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H18">
-        <v>1.023023794416142e-10</v>
+        <v>8.52645742997569e-12</v>
       </c>
       <c r="I18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1108,28 +1096,28 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>2.856724158006863e-05</v>
+        <v>2.903386394415008e-06</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F19" t="s">
         <v>48</v>
       </c>
       <c r="G19" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H19">
-        <v>4.002482387601166e-12</v>
+        <v>3.946807303681269e-12</v>
       </c>
       <c r="I19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1137,28 +1125,28 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>4.529387570340049e-06</v>
+        <v>2.18533886964245e-06</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H20">
-        <v>1.712968376020841e-10</v>
+        <v>1.532501143447098e-13</v>
       </c>
       <c r="I20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1166,28 +1154,28 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>3.436698840619812e-06</v>
+        <v>1.110634883394468e-06</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G21" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H21">
-        <v>3.712051554976899e-13</v>
+        <v>3.424265629235221e-13</v>
       </c>
       <c r="I21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1195,28 +1183,28 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>9.278560082481846e-07</v>
+        <v>8.171932390776959e-07</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H22">
-        <v>1.866058317560418e-12</v>
+        <v>2.556214952645278e-14</v>
       </c>
       <c r="I22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1224,28 +1212,28 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>6.358513142679101e-07</v>
+        <v>1.240146862979685e-07</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G23" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H23">
-        <v>2.546537551127804e-14</v>
+        <v>1.424521215091434e-13</v>
       </c>
       <c r="I23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1253,173 +1241,28 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1.728888672225537e-07</v>
+        <v>2.325140990855346e-08</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G24" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H24">
-        <v>6.35447879014813e-14</v>
+        <v>3.024317889931462e-15</v>
       </c>
       <c r="I24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>1.097154358475905e-07</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25">
-        <v>1.189507658314286e-15</v>
-      </c>
-      <c r="I25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>9.537164769035655e-08</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" t="s">
-        <v>48</v>
-      </c>
-      <c r="G26" t="s">
-        <v>51</v>
-      </c>
-      <c r="H26">
-        <v>6.111462730262687e-17</v>
-      </c>
-      <c r="I26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27">
-        <v>8.274579910150237e-08</v>
-      </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" t="s">
-        <v>51</v>
-      </c>
-      <c r="H27">
-        <v>4.726596440914009e-17</v>
-      </c>
-      <c r="I27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>3.278881033352832e-08</v>
-      </c>
-      <c r="C28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" t="s">
-        <v>51</v>
-      </c>
-      <c r="G28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H28">
-        <v>7.398889152812689e-16</v>
-      </c>
-      <c r="I28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29">
-        <v>1.660658077717869e-08</v>
-      </c>
-      <c r="C29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29">
-        <v>7.770727681979428e-17</v>
-      </c>
-      <c r="I29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>